<commit_message>
update mockup and WBS
</commit_message>
<xml_diff>
--- a/docs/WBS.xlsx
+++ b/docs/WBS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="140">
   <si>
     <t>Owner</t>
   </si>
@@ -452,9 +452,6 @@
     <t>因为使用开发者模式，菜单需要调用接口编程实现</t>
   </si>
   <si>
-    <t>需要抽取“出发日期”，去掉乱码</t>
-  </si>
-  <si>
     <t>显示足迹时，没有标题的足迹不显示</t>
   </si>
   <si>
@@ -487,6 +484,15 @@
   </si>
   <si>
     <t>集成/代码整理</t>
+  </si>
+  <si>
+    <t>需要抽取“出发日期”，去掉乱码
+分段落
+图片存储二进制
+递增抓数据</t>
+  </si>
+  <si>
+    <t>马、刘</t>
   </si>
 </sst>
 </file>
@@ -661,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -747,6 +753,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1173,9 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1358,7 +1365,7 @@
         <v>53</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1457,48 +1464,51 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="28">
+      <c r="E12" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="25">
         <v>41852</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="25">
         <v>41856</v>
       </c>
+      <c r="H12" s="23"/>
       <c r="I12" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="25">
         <v>41852</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="25">
         <v>41855</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="35" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1565,7 +1575,7 @@
       <c r="H16" s="32"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>35</v>
       </c>
@@ -1582,31 +1592,35 @@
         <v>41855</v>
       </c>
       <c r="G17" s="28">
-        <v>41857</v>
+        <v>41858</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="22" t="s">
+      <c r="C18" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="28">
+      <c r="E18" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="25">
         <v>41856</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="25">
         <v>41856</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>36</v>
       </c>
@@ -1621,13 +1635,13 @@
         <v>41857</v>
       </c>
       <c r="G19" s="28">
-        <v>41857</v>
+        <v>41858</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>36</v>
       </c>
@@ -1637,7 +1651,9 @@
       <c r="D20" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="F20" s="28">
         <v>41858</v>
       </c>
@@ -1648,7 +1664,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>36</v>
       </c>
@@ -1672,7 +1688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>36</v>
       </c>
@@ -1696,12 +1712,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>11</v>
@@ -1711,34 +1727,34 @@
         <v>41855</v>
       </c>
       <c r="G23" s="28">
-        <v>41857</v>
+        <v>41858</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="28">
-        <v>41858</v>
+        <v>41859</v>
       </c>
       <c r="G24" s="28">
         <v>41859</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
         <v>36</v>
       </c>
@@ -1757,7 +1773,7 @@
       </c>
       <c r="H25" s="26"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>36</v>
       </c>
@@ -1777,12 +1793,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>23</v>
@@ -1798,7 +1814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
         <v>6</v>
       </c>
@@ -1815,7 +1831,7 @@
         <v>41871</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
         <v>7</v>
       </c>
@@ -2223,12 +2239,12 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2293,12 +2309,12 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2353,7 +2369,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2403,7 +2419,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2504,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,7 +2554,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>